<commit_message>
Add new Cypress test cases and automation script
</commit_message>
<xml_diff>
--- a/Daily_Tracker.xlsx
+++ b/Daily_Tracker.xlsx
@@ -1,43 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaibhav suryawanshi\Desktop\Cypress_Task\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A60640-6B02-48D3-827A-2D3A88C80231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="TestResults" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>Test Case Title</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>01_verify_Adding_single_item_to_cart</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>02_verify_removing_item_from_the_cart</t>
-  </si>
-  <si>
-    <t>03_verify_updating_of_cart_after_adding_multiple_item</t>
+    <t>16-05-2025</t>
+  </si>
+  <si>
+    <t>17-05-2025</t>
+  </si>
+  <si>
+    <t>11_failed</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>07_verify_Adding_single_item_to_cart</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>08_verify_removing_item_from_the_cart</t>
+  </si>
+  <si>
+    <t>09_verify_updating_of_cart_after_adding_multiple_item</t>
   </si>
   <si>
     <t>01_Verify_Valid_Login</t>
@@ -49,34 +52,77 @@
     <t>03_Verify_Lockout_user_failed_login</t>
   </si>
   <si>
-    <t>01_verify_complete_successful_purchase_of_single_item</t>
-  </si>
-  <si>
-    <t>02_verify_checkout_with_missing_firstname_fails.cy.js</t>
-  </si>
-  <si>
-    <t>03_verify_user_can_cancel_checkout_and redirected_to_cart.cy.js</t>
+    <t>04_verify_complete_successful_purchase_of_single_item</t>
+  </si>
+  <si>
+    <t>05_verify_checkout_with_missing_firstname_fails.cy.js</t>
+  </si>
+  <si>
+    <t>06_verify_user_can_cancel_checkout_and redirected_to_cart.cy.js</t>
+  </si>
+  <si>
+    <t>10_verify_complete_successful_purchase_of_single_item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="9C0006"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="006100"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,14 +137,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -431,110 +481,152 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="74.19921875" customWidth="1"/>
+    <col min="1" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:B11" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add github action flow
</commit_message>
<xml_diff>
--- a/Daily_Tracker.xlsx
+++ b/Daily_Tracker.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387A589E-6888-4FED-9D41-3B6B81D2F6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="TestResults" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="TestResults" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Summary" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>Test Case Title</t>
   </si>
@@ -63,43 +63,57 @@
   </si>
   <si>
     <t>10_verify_complete_successful_purchase_of_single_item</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>% Passed</t>
+  </si>
+  <si>
+    <t>91%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <color rgb="FF9C0006"/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <color rgb="9C0006"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF006100"/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <color rgb="006100"/>
     </font>
   </fonts>
   <fills count="6">
@@ -116,7 +130,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -126,7 +140,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -486,14 +500,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="58.5546875" customWidth="1"/>
     <col min="2" max="3" width="20" customWidth="1"/>
@@ -633,6 +647,68 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>